<commit_message>
finished Exploratory Testing For Profile Page
</commit_message>
<xml_diff>
--- a/Documentation/Manual Testing/Profile Page/Exploratory Testing Report [Profile Page].xlsx
+++ b/Documentation/Manual Testing/Profile Page/Exploratory Testing Report [Profile Page].xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24519"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{20D748D8-83F2-414F-A082-7F870479A392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Princ\source\SDETCourseMaterial\SDET_CourseMaterial\Eng91_FinalProject\Documentation\Manual Testing\Profile Page\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A64E03-90FB-4D63-9301-017477BF963C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6045" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,9 +30,107 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="31">
+  <si>
+    <t>TESTS</t>
+  </si>
+  <si>
+    <t>STEPS</t>
+  </si>
+  <si>
+    <t>ACTIONS</t>
+  </si>
+  <si>
+    <t>RESULT / ERROR MESSAGE *</t>
+  </si>
+  <si>
+    <t>Profiles Section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIVEN I am a trainer </t>
+  </si>
+  <si>
+    <t>AND my username is 'jsmith'</t>
+  </si>
+  <si>
+    <t>AND my password is 'Password123!'</t>
+  </si>
+  <si>
+    <t>AND I click on Profiles</t>
+  </si>
+  <si>
+    <t>WHEN I click 'submit'</t>
+  </si>
+  <si>
+    <t>AND i type in the email field 'email@email.com'</t>
+  </si>
+  <si>
+    <t>AND I type in the name field 'name'</t>
+  </si>
+  <si>
+    <t>THEN I should receive a messege or a notification</t>
+  </si>
+  <si>
+    <t>/ logged in as trainer</t>
+  </si>
+  <si>
+    <t>/ logged is as 'jsmith'</t>
+  </si>
+  <si>
+    <t>AND I leave the email field empty</t>
+  </si>
+  <si>
+    <t>AND I leave the name field empty</t>
+  </si>
+  <si>
+    <t>/ empty email field</t>
+  </si>
+  <si>
+    <t>/ empty name field</t>
+  </si>
+  <si>
+    <t>/ 'name' in name field</t>
+  </si>
+  <si>
+    <t>/ email@email.com in email field</t>
+  </si>
+  <si>
+    <t>&gt; no indication of what the Recipient section does</t>
+  </si>
+  <si>
+    <t>&gt; no indication of whether or not the submit button works</t>
+  </si>
+  <si>
+    <t>/ Testing Recipient functionality</t>
+  </si>
+  <si>
+    <t>&gt; SendAccessLink in FrontEnt -&gt; Controllers -&gt; ProfileController.cs</t>
+  </si>
+  <si>
+    <t>&gt; page redirects to itself and returns status code 302 [found]</t>
+  </si>
+  <si>
+    <t>/ checked developer mode -&gt;  network</t>
+  </si>
+  <si>
+    <t>seams to be responsible for POST request from the form data</t>
+  </si>
+  <si>
+    <t>AND I select 'Engineering81' in Courses</t>
+  </si>
+  <si>
+    <t>/ selected 'All Courses' in Courses tab</t>
+  </si>
+  <si>
+    <t>/ selected 'Eng81' in Courses tab</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -35,13 +138,67 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA6A6A6"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -56,14 +213,47 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFB7B7"/>
+      <color rgb="FFFF8585"/>
+      <color rgb="FFFF6969"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -372,14 +562,317 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="27.73046875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="53.796875" customWidth="1"/>
+    <col min="3" max="3" width="39.1328125" customWidth="1"/>
+    <col min="4" max="4" width="63" customWidth="1"/>
+    <col min="6" max="6" width="9.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="4"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="5">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="10"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="8">
+        <v>2</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="8"/>
+      <c r="B15" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="8"/>
+      <c r="B16" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="11"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17" s="8"/>
+      <c r="B17" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="9"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18" s="8"/>
+      <c r="B18" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19" s="8"/>
+      <c r="B19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="9"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A20" s="8"/>
+      <c r="B20" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A21" s="8"/>
+      <c r="B21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="9"/>
+      <c r="D21" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A22" s="8"/>
+      <c r="B22" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25" s="5">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="10"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="10"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B29" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added dev mode info in documentation
</commit_message>
<xml_diff>
--- a/Documentation/Manual Testing/Profile Page/Exploratory Testing Report [Profile Page].xlsx
+++ b/Documentation/Manual Testing/Profile Page/Exploratory Testing Report [Profile Page].xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Princ\source\SDETCourseMaterial\SDET_CourseMaterial\Eng91_FinalProject\Documentation\Manual Testing\Profile Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A64E03-90FB-4D63-9301-017477BF963C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F69CFA-314D-491F-AA40-4FFDA6E3A6A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6045" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -111,9 +111,6 @@
     <t>&gt; page redirects to itself and returns status code 302 [found]</t>
   </si>
   <si>
-    <t>/ checked developer mode -&gt;  network</t>
-  </si>
-  <si>
     <t>seams to be responsible for POST request from the form data</t>
   </si>
   <si>
@@ -124,6 +121,9 @@
   </si>
   <si>
     <t>/ selected 'Eng81' in Courses tab</t>
+  </si>
+  <si>
+    <t>/ CHROME developer mode -&gt;  network</t>
   </si>
 </sst>
 </file>
@@ -564,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -670,10 +670,10 @@
         <v>11</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
@@ -681,7 +681,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>25</v>
@@ -756,20 +756,20 @@
         <v>16</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D19" s="9"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="8"/>
       <c r="B20" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
@@ -849,10 +849,10 @@
         <v>11</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
@@ -860,7 +860,7 @@
         <v>9</v>
       </c>
       <c r="C31" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D31" s="13" t="s">
         <v>25</v>

</xml_diff>